<commit_message>
Aggionramento file report-checklist per errato testo nella colonna gestione errore test 45
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111WECONSTUDIOXX/WECONSTUDIO/CDCSM/1.0/report-checklist.xlsx
+++ b/GATEWAY/S1#111WECONSTUDIOXX/WECONSTUDIO/CDCSM/1.0/report-checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tsclient\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF3E336-6AB5-4BE0-AAEE-9ED81F633B68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A56E73-A9D4-4364-9B33-D1B46AD41FAB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17100" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -812,9 +812,6 @@
     <t>Errore nella fase di validazione del cda2</t>
   </si>
   <si>
-    <t>L'operatore provvede a sistemare i dati e rigenerare manualmente il documento, solo a validazione avvenuta saranno consentiti i passaggi successivi</t>
-  </si>
-  <si>
     <t>Validazione gestita lato applicativo</t>
   </si>
   <si>
@@ -825,6 +822,13 @@
   </si>
   <si>
     <t>2023-09-04T13:54:18Z</t>
+  </si>
+  <si>
+    <t>L’errore viene segnalato a video all’utente finale, raccomandando di riprovare in un secondo momento l’operazione e nel caso non si dovesse risolvere in tempi brevi di contattare l’help-desk aziendale per la risoluzione.
+Il servizio di manutenzione software aziendale, analizzerà giornalmente i log per rilevare questa tipologia di errore ed interverrà autonomamente, o sotto richiesta dell’help-desk, per la risoluzione dell’errore.
+Risolto l’errore, il medico sarà contattato per riprendere il processo documentale dal punto in cui si era bloccato al fine di consentire il re-invio al gateway per la validazione.
+Se il Gateway non fosse disponibile in fase di validazione il processo clinico prosegue, il documento verrà memorizzato nel DataBase aziendale ed al ripristinarsi del servizio il documento re-inviato al gateway per la validazione e successivi step di invio al Repository Aziendale e al FSE regionale.
+Per quanto riguarda gli errori di timeout non sono previste code di reinvio automatico. Ogni errore sarà gestito puntualmente come sopra descritto.</t>
   </si>
 </sst>
 </file>
@@ -1282,6 +1286,9 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1291,6 +1298,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1303,12 +1313,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1622,7 +1626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -3789,11 +3793,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T646"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="M10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="9" topLeftCell="J15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="H36" sqref="H36"/>
+      <selection pane="bottomRight" activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -3832,14 +3836,14 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="18.75">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="44" t="s">
+      <c r="B2" s="44"/>
+      <c r="C2" s="45" t="s">
         <v>157</v>
       </c>
-      <c r="D2" s="52"/>
+      <c r="D2" s="46"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -3857,14 +3861,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="15.75">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="51" t="s">
+      <c r="B3" s="48"/>
+      <c r="C3" s="53" t="s">
         <v>158</v>
       </c>
-      <c r="D3" s="43"/>
+      <c r="D3" s="44"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -3882,12 +3886,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="15.75">
-      <c r="A4" s="47"/>
-      <c r="B4" s="48"/>
-      <c r="C4" s="51" t="s">
+      <c r="A4" s="49"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="53" t="s">
         <v>159</v>
       </c>
-      <c r="D4" s="43"/>
+      <c r="D4" s="44"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -3906,12 +3910,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="15.75">
-      <c r="A5" s="49"/>
-      <c r="B5" s="50"/>
-      <c r="C5" s="51" t="s">
+      <c r="A5" s="51"/>
+      <c r="B5" s="52"/>
+      <c r="C5" s="53" t="s">
         <v>147</v>
       </c>
-      <c r="D5" s="43"/>
+      <c r="D5" s="44"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -3929,8 +3933,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="40"/>
-      <c r="B6" s="41"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="42"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4275,7 +4279,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="90.75" thickBot="1">
+    <row r="16" spans="1:20" ht="60.75" thickBot="1">
       <c r="A16" s="35">
         <v>45</v>
       </c>
@@ -4307,14 +4311,14 @@
       <c r="M16" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="N16" s="53" t="s">
+      <c r="N16" s="40" t="s">
         <v>160</v>
       </c>
       <c r="O16" s="24" t="s">
         <v>65</v>
       </c>
       <c r="P16" s="38" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="Q16" s="24"/>
       <c r="R16" s="25"/>
@@ -4385,7 +4389,7 @@
         <v>146</v>
       </c>
       <c r="K18" s="38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L18" s="24"/>
       <c r="M18" s="24"/>
@@ -4423,7 +4427,7 @@
         <v>146</v>
       </c>
       <c r="K19" s="38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L19" s="24"/>
       <c r="M19" s="24"/>
@@ -4461,7 +4465,7 @@
         <v>146</v>
       </c>
       <c r="K20" s="38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L20" s="24"/>
       <c r="M20" s="24"/>
@@ -4499,7 +4503,7 @@
         <v>146</v>
       </c>
       <c r="K21" s="38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L21" s="24"/>
       <c r="M21" s="24"/>
@@ -4537,7 +4541,7 @@
         <v>146</v>
       </c>
       <c r="K22" s="38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L22" s="24"/>
       <c r="M22" s="24"/>
@@ -4575,7 +4579,7 @@
         <v>146</v>
       </c>
       <c r="K23" s="38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L23" s="24"/>
       <c r="M23" s="24"/>
@@ -4613,7 +4617,7 @@
         <v>146</v>
       </c>
       <c r="K24" s="38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="L24" s="24"/>
       <c r="M24" s="24"/>
@@ -4799,13 +4803,13 @@
         <v>45173</v>
       </c>
       <c r="G29" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="H29" s="37" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I29" s="37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J29" s="24" t="s">
         <v>65</v>

</xml_diff>